<commit_message>
replaced '..' -> '-'
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/example.xlsx
+++ b/src/test/resources/testdata/example.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="sheet1 1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -84,10 +84,10 @@
     <t>price</t>
   </si>
   <si>
-    <t>1..4</t>
-  </si>
-  <si>
-    <t>5..8</t>
+    <t>1-4</t>
+  </si>
+  <si>
+    <t>5-8</t>
   </si>
   <si>
     <t>test.example.data.Job</t>
@@ -108,7 +108,7 @@
     <t>FLEXIBLE_HOUSING</t>
   </si>
   <si>
-    <t>3..8</t>
+    <t>3-8</t>
   </si>
   <si>
     <t>EVER_LASTING</t>
@@ -133,6 +133,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -154,24 +155,28 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF9900"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -228,7 +233,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -254,14 +259,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -349,17 +346,20 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.6734693877551"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8367346938776"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5561224489796"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1326530612245"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="12.4081632653061"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.6734693877551"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4081632653061"/>
     <col collapsed="false" hidden="false" max="10" min="9" style="0" width="16.7857142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.6734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,10 +1103,13 @@
   <dimension ref="B3:M39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
+      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.6734693877551"/>
+  </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1"/>
@@ -1136,7 +1139,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="7"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
@@ -1160,7 +1163,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="7"/>
+      <c r="M5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="n">
@@ -1186,7 +1189,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="8"/>
+      <c r="M6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="n">
@@ -1215,7 +1218,7 @@
       <c r="K7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="7"/>
+      <c r="M7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
@@ -1246,7 +1249,7 @@
       <c r="K8" s="5" t="n">
         <v>21000</v>
       </c>
-      <c r="M8" s="7"/>
+      <c r="M8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="n">
@@ -1275,7 +1278,7 @@
       <c r="K9" s="5" t="n">
         <v>21000</v>
       </c>
-      <c r="M9" s="7"/>
+      <c r="M9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="n">
@@ -1306,7 +1309,7 @@
       <c r="K10" s="5" t="n">
         <v>33600</v>
       </c>
-      <c r="M10" s="7"/>
+      <c r="M10" s="2"/>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="n">
@@ -1335,7 +1338,7 @@
       <c r="K11" s="5" t="n">
         <v>12600</v>
       </c>
-      <c r="M11" s="7"/>
+      <c r="M11" s="2"/>
     </row>
     <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="n">
@@ -1366,7 +1369,7 @@
       <c r="K12" s="5" t="n">
         <v>21000</v>
       </c>
-      <c r="M12" s="7"/>
+      <c r="M12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="n">
@@ -1395,7 +1398,7 @@
       <c r="K13" s="5" t="n">
         <v>21000</v>
       </c>
-      <c r="M13" s="7"/>
+      <c r="M13" s="2"/>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2"/>
@@ -1416,7 +1419,7 @@
       <c r="K14" s="5" t="n">
         <v>25200</v>
       </c>
-      <c r="M14" s="7"/>
+      <c r="M14" s="2"/>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
@@ -1439,7 +1442,7 @@
       <c r="K15" s="5" t="n">
         <v>12600</v>
       </c>
-      <c r="M15" s="7"/>
+      <c r="M15" s="2"/>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
@@ -1461,7 +1464,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="5"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="7"/>
+      <c r="M16" s="2"/>
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="n">
@@ -1481,7 +1484,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="5"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="7"/>
+      <c r="M17" s="2"/>
     </row>
     <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="n">
@@ -1503,7 +1506,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="7"/>
+      <c r="M18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="n">
@@ -1523,7 +1526,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="7"/>
+      <c r="M19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="n">
@@ -1545,7 +1548,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="7"/>
+      <c r="M20" s="2"/>
     </row>
     <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2"/>
@@ -1559,7 +1562,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="7"/>
+      <c r="M21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2"/>
@@ -1573,7 +1576,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="7"/>
+      <c r="M22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
@@ -1589,7 +1592,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="7"/>
+      <c r="M23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
@@ -1607,7 +1610,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="7"/>
+      <c r="M24" s="2"/>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
@@ -1625,7 +1628,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="M25" s="7"/>
+      <c r="M25" s="2"/>
     </row>
     <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
@@ -1643,7 +1646,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="7"/>
+      <c r="M26" s="2"/>
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2"/>
@@ -1657,7 +1660,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="7"/>
+      <c r="M27" s="2"/>
     </row>
     <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2"/>
@@ -1671,7 +1674,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="7"/>
+      <c r="M28" s="2"/>
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
@@ -1687,7 +1690,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="7"/>
+      <c r="M29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="3" t="s">
@@ -1705,13 +1708,13 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="7"/>
+      <c r="M30" s="2"/>
     </row>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C31" s="9" t="s">
+      <c r="C31" s="7" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="2"/>
@@ -1725,7 +1728,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="7"/>
+      <c r="M31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="n">
@@ -1743,7 +1746,7 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="7"/>
+      <c r="M32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="n">
@@ -1761,7 +1764,7 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="7"/>
+      <c r="M33" s="2"/>
     </row>
     <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="2"/>
@@ -1775,7 +1778,7 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
-      <c r="M34" s="7"/>
+      <c r="M34" s="2"/>
     </row>
     <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
@@ -1791,7 +1794,7 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
-      <c r="M35" s="7"/>
+      <c r="M35" s="2"/>
     </row>
     <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="3" t="s">
@@ -1809,7 +1812,7 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
-      <c r="M36" s="7"/>
+      <c r="M36" s="2"/>
     </row>
     <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="2" t="n">

</xml_diff>

<commit_message>
reverted back to '..'  format
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/example.xlsx
+++ b/src/test/resources/testdata/example.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="sheet1 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="sheet1" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="sheet2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
@@ -84,10 +84,10 @@
     <t>price</t>
   </si>
   <si>
-    <t>1-4</t>
-  </si>
-  <si>
-    <t>5-8</t>
+    <t>1..4</t>
+  </si>
+  <si>
+    <t>5..8</t>
   </si>
   <si>
     <t>test.example.data.Job</t>
@@ -108,7 +108,7 @@
     <t>FLEXIBLE_HOUSING</t>
   </si>
   <si>
-    <t>3-8</t>
+    <t>3..8</t>
   </si>
   <si>
     <t>EVER_LASTING</t>
@@ -133,7 +133,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -155,28 +154,24 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFF9900"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="4">
@@ -233,7 +228,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -259,6 +254,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -346,20 +349,17 @@
   <dimension ref="A1:L36"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B36" activeCellId="0" sqref="B36"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.6734693877551"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.8367346938776"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.5561224489796"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.1326530612245"/>
     <col collapsed="false" hidden="false" max="6" min="5" style="0" width="12.4081632653061"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.6734693877551"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="12.4081632653061"/>
     <col collapsed="false" hidden="false" max="10" min="9" style="0" width="16.7857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="0" width="8.6734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1103,13 +1103,10 @@
   <dimension ref="B3:M39"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B39" activeCellId="0" sqref="B39"/>
+      <selection pane="topLeft" activeCell="K8" activeCellId="0" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.6734693877551"/>
-  </cols>
   <sheetData>
     <row r="3" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="1"/>
@@ -1139,7 +1136,7 @@
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="M4" s="7"/>
     </row>
     <row r="5" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="3" t="s">
@@ -1163,7 +1160,7 @@
       <c r="J5" s="2"/>
       <c r="K5" s="2"/>
       <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="M5" s="7"/>
     </row>
     <row r="6" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="n">
@@ -1189,7 +1186,7 @@
       <c r="J6" s="2"/>
       <c r="K6" s="2"/>
       <c r="L6" s="2"/>
-      <c r="M6" s="4"/>
+      <c r="M6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="n">
@@ -1218,7 +1215,7 @@
       <c r="K7" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="M7" s="2"/>
+      <c r="M7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
@@ -1249,7 +1246,7 @@
       <c r="K8" s="5" t="n">
         <v>21000</v>
       </c>
-      <c r="M8" s="2"/>
+      <c r="M8" s="7"/>
     </row>
     <row r="9" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="n">
@@ -1278,7 +1275,7 @@
       <c r="K9" s="5" t="n">
         <v>21000</v>
       </c>
-      <c r="M9" s="2"/>
+      <c r="M9" s="7"/>
     </row>
     <row r="10" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="n">
@@ -1309,7 +1306,7 @@
       <c r="K10" s="5" t="n">
         <v>33600</v>
       </c>
-      <c r="M10" s="2"/>
+      <c r="M10" s="7"/>
     </row>
     <row r="11" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="n">
@@ -1338,7 +1335,7 @@
       <c r="K11" s="5" t="n">
         <v>12600</v>
       </c>
-      <c r="M11" s="2"/>
+      <c r="M11" s="7"/>
     </row>
     <row r="12" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="n">
@@ -1369,7 +1366,7 @@
       <c r="K12" s="5" t="n">
         <v>21000</v>
       </c>
-      <c r="M12" s="2"/>
+      <c r="M12" s="7"/>
     </row>
     <row r="13" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="n">
@@ -1398,7 +1395,7 @@
       <c r="K13" s="5" t="n">
         <v>21000</v>
       </c>
-      <c r="M13" s="2"/>
+      <c r="M13" s="7"/>
     </row>
     <row r="14" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2"/>
@@ -1419,7 +1416,7 @@
       <c r="K14" s="5" t="n">
         <v>25200</v>
       </c>
-      <c r="M14" s="2"/>
+      <c r="M14" s="7"/>
     </row>
     <row r="15" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="1" t="s">
@@ -1442,7 +1439,7 @@
       <c r="K15" s="5" t="n">
         <v>12600</v>
       </c>
-      <c r="M15" s="2"/>
+      <c r="M15" s="7"/>
     </row>
     <row r="16" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="3" t="s">
@@ -1464,7 +1461,7 @@
       <c r="J16" s="2"/>
       <c r="K16" s="5"/>
       <c r="L16" s="2"/>
-      <c r="M16" s="2"/>
+      <c r="M16" s="7"/>
     </row>
     <row r="17" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="n">
@@ -1484,7 +1481,7 @@
       <c r="J17" s="2"/>
       <c r="K17" s="5"/>
       <c r="L17" s="2"/>
-      <c r="M17" s="2"/>
+      <c r="M17" s="7"/>
     </row>
     <row r="18" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="n">
@@ -1506,7 +1503,7 @@
       <c r="J18" s="2"/>
       <c r="K18" s="2"/>
       <c r="L18" s="2"/>
-      <c r="M18" s="2"/>
+      <c r="M18" s="7"/>
     </row>
     <row r="19" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="n">
@@ -1526,7 +1523,7 @@
       <c r="J19" s="2"/>
       <c r="K19" s="2"/>
       <c r="L19" s="2"/>
-      <c r="M19" s="2"/>
+      <c r="M19" s="7"/>
     </row>
     <row r="20" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="n">
@@ -1548,7 +1545,7 @@
       <c r="J20" s="2"/>
       <c r="K20" s="2"/>
       <c r="L20" s="2"/>
-      <c r="M20" s="2"/>
+      <c r="M20" s="7"/>
     </row>
     <row r="21" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2"/>
@@ -1562,7 +1559,7 @@
       <c r="J21" s="2"/>
       <c r="K21" s="2"/>
       <c r="L21" s="2"/>
-      <c r="M21" s="2"/>
+      <c r="M21" s="7"/>
     </row>
     <row r="22" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2"/>
@@ -1576,7 +1573,7 @@
       <c r="J22" s="2"/>
       <c r="K22" s="2"/>
       <c r="L22" s="2"/>
-      <c r="M22" s="2"/>
+      <c r="M22" s="7"/>
     </row>
     <row r="23" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="1" t="s">
@@ -1592,7 +1589,7 @@
       <c r="J23" s="2"/>
       <c r="K23" s="2"/>
       <c r="L23" s="2"/>
-      <c r="M23" s="2"/>
+      <c r="M23" s="7"/>
     </row>
     <row r="24" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="3" t="s">
@@ -1610,7 +1607,7 @@
       <c r="J24" s="2"/>
       <c r="K24" s="2"/>
       <c r="L24" s="2"/>
-      <c r="M24" s="2"/>
+      <c r="M24" s="7"/>
     </row>
     <row r="25" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="s">
@@ -1628,7 +1625,7 @@
       <c r="J25" s="2"/>
       <c r="K25" s="2"/>
       <c r="L25" s="2"/>
-      <c r="M25" s="2"/>
+      <c r="M25" s="7"/>
     </row>
     <row r="26" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="s">
@@ -1646,7 +1643,7 @@
       <c r="J26" s="2"/>
       <c r="K26" s="2"/>
       <c r="L26" s="2"/>
-      <c r="M26" s="2"/>
+      <c r="M26" s="7"/>
     </row>
     <row r="27" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2"/>
@@ -1660,7 +1657,7 @@
       <c r="J27" s="2"/>
       <c r="K27" s="2"/>
       <c r="L27" s="2"/>
-      <c r="M27" s="2"/>
+      <c r="M27" s="7"/>
     </row>
     <row r="28" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2"/>
@@ -1674,7 +1671,7 @@
       <c r="J28" s="2"/>
       <c r="K28" s="2"/>
       <c r="L28" s="2"/>
-      <c r="M28" s="2"/>
+      <c r="M28" s="7"/>
     </row>
     <row r="29" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="1" t="s">
@@ -1690,7 +1687,7 @@
       <c r="J29" s="2"/>
       <c r="K29" s="2"/>
       <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
+      <c r="M29" s="7"/>
     </row>
     <row r="30" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="3" t="s">
@@ -1708,13 +1705,13 @@
       <c r="J30" s="2"/>
       <c r="K30" s="2"/>
       <c r="L30" s="2"/>
-      <c r="M30" s="2"/>
+      <c r="M30" s="7"/>
     </row>
     <row r="31" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="n">
         <v>1</v>
       </c>
-      <c r="C31" s="7" t="s">
+      <c r="C31" s="9" t="s">
         <v>32</v>
       </c>
       <c r="D31" s="2"/>
@@ -1728,7 +1725,7 @@
       <c r="J31" s="2"/>
       <c r="K31" s="2"/>
       <c r="L31" s="2"/>
-      <c r="M31" s="2"/>
+      <c r="M31" s="7"/>
     </row>
     <row r="32" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="n">
@@ -1746,7 +1743,7 @@
       <c r="J32" s="2"/>
       <c r="K32" s="2"/>
       <c r="L32" s="2"/>
-      <c r="M32" s="2"/>
+      <c r="M32" s="7"/>
     </row>
     <row r="33" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="n">
@@ -1764,7 +1761,7 @@
       <c r="J33" s="2"/>
       <c r="K33" s="2"/>
       <c r="L33" s="2"/>
-      <c r="M33" s="2"/>
+      <c r="M33" s="7"/>
     </row>
     <row r="34" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="2"/>
@@ -1778,7 +1775,7 @@
       <c r="J34" s="2"/>
       <c r="K34" s="2"/>
       <c r="L34" s="2"/>
-      <c r="M34" s="2"/>
+      <c r="M34" s="7"/>
     </row>
     <row r="35" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="1" t="s">
@@ -1794,7 +1791,7 @@
       <c r="J35" s="2"/>
       <c r="K35" s="2"/>
       <c r="L35" s="2"/>
-      <c r="M35" s="2"/>
+      <c r="M35" s="7"/>
     </row>
     <row r="36" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="3" t="s">
@@ -1812,7 +1809,7 @@
       <c r="J36" s="2"/>
       <c r="K36" s="2"/>
       <c r="L36" s="2"/>
-      <c r="M36" s="2"/>
+      <c r="M36" s="7"/>
     </row>
     <row r="37" customFormat="false" ht="14.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="2" t="n">

</xml_diff>